<commit_message>
Completed translation of 集会所 ★7 quest title.
</commit_message>
<xml_diff>
--- a/data_M.xlsx
+++ b/data_M.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3325" uniqueCount="1073">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3400" uniqueCount="1145">
   <si>
     <t>questName</t>
   </si>
@@ -2593,6 +2593,9 @@
     <t>鎚と刀の鍔迫り合い</t>
   </si>
   <si>
+    <t>철퇴와 칼의 치열한 접전</t>
+  </si>
+  <si>
     <t>집회소★7</t>
   </si>
   <si>
@@ -2611,6 +2614,9 @@
     <t>住めば都の闘技場暮らし</t>
   </si>
   <si>
+    <t>정들면 고향인 투기장 생활</t>
+  </si>
+  <si>
     <t>闘技場</t>
   </si>
   <si>
@@ -2620,6 +2626,9 @@
     <t>熱気で熱狂！炎の軍勢！</t>
   </si>
   <si>
+    <t>열기로 열광! 불꽃의 군세!</t>
+  </si>
+  <si>
     <t>3700z</t>
   </si>
   <si>
@@ -2629,6 +2638,9 @@
     <t>蒼く渦巻く登竜門</t>
   </si>
   <si>
+    <t>파랗게 소용돌이치는 등용문</t>
+  </si>
+  <si>
     <t>渓流</t>
   </si>
   <si>
@@ -2641,6 +2653,9 @@
     <t>灼熱砂上の荒ぶる刀剣</t>
   </si>
   <si>
+    <t>작열의 모래 위의 난폭한 도검</t>
+  </si>
+  <si>
     <t>旧砂漠</t>
   </si>
   <si>
@@ -2653,6 +2668,9 @@
     <t>月夜に出でし阿吽の雷撃</t>
   </si>
   <si>
+    <t>달밤에 나타난 아훔의 뇌격</t>
+  </si>
+  <si>
     <t>古代林</t>
   </si>
   <si>
@@ -2668,6 +2686,9 @@
     <t>憤怒の雄叫び</t>
   </si>
   <si>
+    <t>분노의 포효</t>
+  </si>
+  <si>
     <t>怒り喰らうイビルジョー1頭の狩猟</t>
   </si>
   <si>
@@ -2677,6 +2698,9 @@
     <t>金獅子の黒き覇気</t>
   </si>
   <si>
+    <t>금사자의 검은 패기</t>
+  </si>
+  <si>
     <t>ラージャン1頭の狩猟</t>
   </si>
   <si>
@@ -2686,6 +2710,9 @@
     <t>荒れる山神、鎮める狩人</t>
   </si>
   <si>
+    <t>날뛰는 산신, 진정시키는 사냥꾼</t>
+  </si>
+  <si>
     <t>雪山</t>
   </si>
   <si>
@@ -2698,6 +2725,9 @@
     <t>竜のコリーダ</t>
   </si>
   <si>
+    <t>용의 투우</t>
+  </si>
+  <si>
     <t>立体闘技場</t>
   </si>
   <si>
@@ -2707,6 +2737,9 @@
     <t>震天動地なグランドウイング</t>
   </si>
   <si>
+    <t>경천동지할 그랜드 윙</t>
+  </si>
+  <si>
     <t>乗りによるダウンを5回成功</t>
   </si>
   <si>
@@ -2731,6 +2764,9 @@
     <t>竜王の系譜</t>
   </si>
   <si>
+    <t>용왕의 계보</t>
+  </si>
+  <si>
     <t>リオレウス希少種1頭とリオレイア希少種1頭の狩猟</t>
   </si>
   <si>
@@ -2740,12 +2776,18 @@
     <t>受付嬢オススメ！雷狼竜×２</t>
   </si>
   <si>
+    <t>여성 접수원의 추천! 뇌랑룡×2</t>
+  </si>
+  <si>
     <t>ジンオウガ2頭の狩猟</t>
   </si>
   <si>
     <t>超☆メモ帳～千刃竜捕獲編～</t>
   </si>
   <si>
+    <t>초☆메모장 ~천인룡포획편~</t>
+  </si>
+  <si>
     <t>セルレギオス1頭の捕獲</t>
   </si>
   <si>
@@ -2755,6 +2797,9 @@
     <t>柔能く剛能く狩人を制す</t>
   </si>
   <si>
+    <t>부드럽고 유연하고 강한자야 말로 사냥꾼을 제압할 수 있다. (유능제강의 언어유희)</t>
+  </si>
+  <si>
     <t>タマミツネ1頭の狩猟</t>
   </si>
   <si>
@@ -2764,6 +2809,9 @@
     <t>湯けむりと噴煙と</t>
   </si>
   <si>
+    <t>수증기와 분연과</t>
+  </si>
+  <si>
     <t>火山</t>
   </si>
   <si>
@@ -2776,6 +2824,9 @@
     <t>絶対零度</t>
   </si>
   <si>
+    <t>절대영도</t>
+  </si>
+  <si>
     <t>極圏</t>
   </si>
   <si>
@@ -2794,6 +2845,9 @@
     <t>熱愛発覚！？竜達の密会！</t>
   </si>
   <si>
+    <t>열애발각!? 용들의 밀회!</t>
+  </si>
+  <si>
     <t>遺跡平原</t>
   </si>
   <si>
@@ -2803,6 +2857,9 @@
     <t>黄金の月輪</t>
   </si>
   <si>
+    <t>황금의 월륜</t>
+  </si>
+  <si>
     <t>リオレイア希少種1頭の狩猟</t>
   </si>
   <si>
@@ -2812,6 +2869,9 @@
     <t>山紫水明の破壊者</t>
   </si>
   <si>
+    <t>산자수명한 파괴자</t>
+  </si>
+  <si>
     <t>ドボルベルク1頭の狩猟</t>
   </si>
   <si>
@@ -2821,6 +2881,9 @@
     <t>電光煌めく飛竜の夜</t>
   </si>
   <si>
+    <t>전광이 빛나는 비룡의 밤</t>
+  </si>
+  <si>
     <t>ライゼクス1頭の狩猟</t>
   </si>
   <si>
@@ -2830,6 +2893,9 @@
     <t>熱き闘魂、纏いし炎戈</t>
   </si>
   <si>
+    <t>뜨거운 투혼, 휘감은 염과</t>
+  </si>
+  <si>
     <t>アグナコトル1頭の狩猟</t>
   </si>
   <si>
@@ -2839,6 +2905,9 @@
     <t>戦々恐々、最恐コンビ</t>
   </si>
   <si>
+    <t>전전긍긍, 가장 두려운 콤비</t>
+  </si>
+  <si>
     <t>イビルジョー1頭とラージャン1頭の狩猟</t>
   </si>
   <si>
@@ -2848,6 +2917,9 @@
     <t>奈落の妖星</t>
   </si>
   <si>
+    <t>나락의 요성</t>
+  </si>
+  <si>
     <t>竜ノ墓場</t>
   </si>
   <si>
@@ -2857,6 +2929,9 @@
     <t>轟虎馮海</t>
   </si>
   <si>
+    <t>굉호풍해</t>
+  </si>
+  <si>
     <t>氷海</t>
   </si>
   <si>
@@ -2869,27 +2944,42 @@
     <t>奇奇怪怪のハードビーク</t>
   </si>
   <si>
+    <t>기기괴괴의 하드비크</t>
+  </si>
+  <si>
     <t>17100z</t>
   </si>
   <si>
     <t>破壊と滅亡の申し子</t>
   </si>
   <si>
+    <t>파괴와 멸망의 산물</t>
+  </si>
+  <si>
     <t>曇天毒雨</t>
   </si>
   <si>
+    <t>담천독우</t>
+  </si>
+  <si>
     <t>ガブラス20頭の討伐</t>
   </si>
   <si>
     <t>ビリビリバリバリパニック！！</t>
   </si>
   <si>
+    <t>비리비리바리바리패닉!!</t>
+  </si>
+  <si>
     <t>38700z</t>
   </si>
   <si>
     <t>ユクモノ足湯と雷狼竜</t>
   </si>
   <si>
+    <t>유쿠모의 족욕과 뇌랑룡</t>
+  </si>
+  <si>
     <t>孤島</t>
   </si>
   <si>
@@ -2902,6 +2992,9 @@
     <t>凶賊ゲリョス狩り</t>
   </si>
   <si>
+    <t>흉적 게료스 사냥</t>
+  </si>
+  <si>
     <t>沼地</t>
   </si>
   <si>
@@ -2911,6 +3004,9 @@
     <t>昂ぶる千の刃</t>
   </si>
   <si>
+    <t>고조되는 천의 칼날</t>
+  </si>
+  <si>
     <t>セルレギオス1頭の狩猟</t>
   </si>
   <si>
@@ -2920,6 +3016,9 @@
     <t>遺跡平原からの伝書</t>
   </si>
   <si>
+    <t>유적평원으로부터의 전서</t>
+  </si>
+  <si>
     <t>イビルジョー1頭の狩猟</t>
   </si>
   <si>
@@ -2929,6 +3028,9 @@
     <t>試練の帰結点</t>
   </si>
   <si>
+    <t>시련의 귀결점</t>
+  </si>
+  <si>
     <t>乗りによるダウンを4回成功</t>
   </si>
   <si>
@@ -2938,6 +3040,9 @@
     <t>容赦なき、金獅子相手に用心棒</t>
   </si>
   <si>
+    <t>용서없는, 금사자 상대로 경호원</t>
+  </si>
+  <si>
     <t>ラージャン3頭の狩猟</t>
   </si>
   <si>
@@ -2953,6 +3058,9 @@
     <t>吹き荒れる災厄の火</t>
   </si>
   <si>
+    <t>휘몰아치는 재액의 불</t>
+  </si>
+  <si>
     <t>テオ・テスカトルの討伐または撃退</t>
   </si>
   <si>
@@ -2962,6 +3070,9 @@
     <t>白と瑠璃の輪舞曲</t>
   </si>
   <si>
+    <t>백과 유리의 윤무곡</t>
+  </si>
+  <si>
     <t>原生林</t>
   </si>
   <si>
@@ -2974,12 +3085,18 @@
     <t>千刃竜セルレギオス</t>
   </si>
   <si>
+    <t>천인룡 셀레기오스</t>
+  </si>
+  <si>
     <t>乗りよるダウンを2回成功</t>
   </si>
   <si>
     <t>舞うは嵐、奏でるは災禍の調べ</t>
   </si>
   <si>
+    <t>춤추면 태풍, 연주하면 재화의 조사</t>
+  </si>
+  <si>
     <t>霊峰</t>
   </si>
   <si>
@@ -2992,6 +3109,9 @@
     <t>いつか見た幻日</t>
   </si>
   <si>
+    <t>언젠가 보았던 환일</t>
+  </si>
+  <si>
     <t>リオレウス希少種1頭の狩猟</t>
   </si>
   <si>
@@ -3004,27 +3124,42 @@
     <t>舞い降りる鋼龍</t>
   </si>
   <si>
+    <t>훨훨 내려앉은 강룡</t>
+  </si>
+  <si>
     <t>クシャルダオラの翼破壊</t>
   </si>
   <si>
     <t>白銀の火輪</t>
   </si>
   <si>
+    <t>백은의 화륜</t>
+  </si>
+  <si>
     <t>リオレウス希少種の頭部破壊</t>
   </si>
   <si>
     <t>モンスターニャンター</t>
   </si>
   <si>
+    <t>몬스터 냥타</t>
+  </si>
+  <si>
     <t>天に吼えろ、大地を揺らせ</t>
   </si>
   <si>
+    <t>하늘에 짖고, 대지를 울려라</t>
+  </si>
+  <si>
     <t>ジンオウガ1頭とティガレックス1頭の狩猟</t>
   </si>
   <si>
     <t>森丘の黒い霧</t>
   </si>
   <si>
+    <t>숲과언덕의 검은 안개</t>
+  </si>
+  <si>
     <t>竜の大粒ナミダ2個の納品</t>
   </si>
   <si>
@@ -3034,6 +3169,9 @@
     <t>顕現せし黒蝕竜</t>
   </si>
   <si>
+    <t>현현한 흑식룡</t>
+  </si>
+  <si>
     <t>ゴア・マガラ1頭の狩猟</t>
   </si>
   <si>
@@ -3046,6 +3184,9 @@
     <t>獰にして猛だが火でもある</t>
   </si>
   <si>
+    <t>영에 맹이지만 불이기도 하다</t>
+  </si>
+  <si>
     <t>リオレウス1頭の狩猟</t>
   </si>
   <si>
@@ -3055,12 +3196,18 @@
     <t>痺れる魔球</t>
   </si>
   <si>
+    <t>저리는 마구</t>
+  </si>
+  <si>
     <t>ラングロトラ1頭の狩猟</t>
   </si>
   <si>
     <t>縦横無尽なフレックスフィン</t>
   </si>
   <si>
+    <t>종횡무진한 플렉스핀</t>
+  </si>
+  <si>
     <t>水上闘技場</t>
   </si>
   <si>
@@ -3073,21 +3220,33 @@
     <t>グランド・ハンター・ゲーム</t>
   </si>
   <si>
+    <t>그랜드・헌터・게임</t>
+  </si>
+  <si>
     <t>アルセルタスを除く全ての大型モンスターの狩猟</t>
   </si>
   <si>
     <t>原生林の平和を守れ</t>
   </si>
   <si>
+    <t>원시림의 평화를 지켜라</t>
+  </si>
+  <si>
     <t>20100z</t>
   </si>
   <si>
     <t>勇猛果敢なブレイブタスク</t>
   </si>
   <si>
+    <t>용맹과감한 브레이브 태스크</t>
+  </si>
+  <si>
     <t>難攻不落の重甲虫</t>
   </si>
   <si>
+    <t>난공불략의 중갑충</t>
+  </si>
+  <si>
     <t>ゲネル・セルタス1匹の狩猟</t>
   </si>
   <si>
@@ -3097,6 +3256,9 @@
     <t>鎧袖一触のパワフルアームズ</t>
   </si>
   <si>
+    <t>개수일촉의 파워풀 암즈</t>
+  </si>
+  <si>
     <t>4000z</t>
   </si>
   <si>
@@ -3109,6 +3271,9 @@
     <t>冷たき甲冑</t>
   </si>
   <si>
+    <t>차가운 갑주</t>
+  </si>
+  <si>
     <t>ガムート1頭とザボアザギル1頭の狩猟</t>
   </si>
   <si>
@@ -3118,9 +3283,15 @@
     <t>炸裂！爆砕拳！</t>
   </si>
   <si>
+    <t>작렬! 폭쇄권!</t>
+  </si>
+  <si>
     <t>彼の地に集いし破滅の禍難</t>
   </si>
   <si>
+    <t>그의 땅에 모여든 파멸의 재난</t>
+  </si>
+  <si>
     <t>禁足地</t>
   </si>
   <si>
@@ -3133,18 +3304,27 @@
     <t>その腕前、噂通りかしら…？</t>
   </si>
   <si>
+    <t>그 솜씨, 소문대로일까나...?</t>
+  </si>
+  <si>
     <t>ディアブロス1頭の狩猟</t>
   </si>
   <si>
     <t>しじまの向こう</t>
   </si>
   <si>
+    <t>침묵의 저편</t>
+  </si>
+  <si>
     <t>オオナズチの尻尾切断</t>
   </si>
   <si>
     <t>灼熱と妖艶</t>
   </si>
   <si>
+    <t>작열과 요염</t>
+  </si>
+  <si>
     <t>塔の秘境</t>
   </si>
   <si>
@@ -3154,6 +3334,9 @@
     <t>煌黒龍アルバトリオン</t>
   </si>
   <si>
+    <t>황흑룡 알바트리온</t>
+  </si>
+  <si>
     <t>溶岩島</t>
   </si>
   <si>
@@ -3166,12 +3349,18 @@
     <t>爆鎚竜の顎破壊に挑戦！</t>
   </si>
   <si>
+    <t>폭추룡의 턱 파괴에 도전!</t>
+  </si>
+  <si>
     <t>ウラガンキンの顎破壊</t>
   </si>
   <si>
     <t>金と銀の煌き</t>
   </si>
   <si>
+    <t>금과 은의 번쩍임</t>
+  </si>
+  <si>
     <t>乗りによるダウンを3回成功</t>
   </si>
   <si>
@@ -3181,12 +3370,18 @@
     <t>まだ見ぬ秘湯をもとめて</t>
   </si>
   <si>
+    <t>아직 보지 못한 비탕을 찾아서</t>
+  </si>
+  <si>
     <t>ジンオウガの頭部と前脚破壊</t>
   </si>
   <si>
     <t>汝ノチカラヲ、見セテミヨ</t>
   </si>
   <si>
+    <t>그대의 힘을, 보여주어보아라</t>
+  </si>
+  <si>
     <t>2800z</t>
   </si>
   <si>
@@ -3196,27 +3391,42 @@
     <t>渓流からの救援要請</t>
   </si>
   <si>
+    <t>계류로부터의 구원요청</t>
+  </si>
+  <si>
     <t>リオレイア希少種の頭部と翼破壊</t>
   </si>
   <si>
     <t>山神と電影</t>
   </si>
   <si>
+    <t>산신과 전영</t>
+  </si>
+  <si>
     <t>ライゼクス1頭とガムート1頭の狩猟</t>
   </si>
   <si>
     <t>空の飛竜と陸の飛竜</t>
   </si>
   <si>
+    <t>하늘의 비룡과 육지의 비룡</t>
+  </si>
+  <si>
     <t>リオレウス1頭とリオレイア1頭の狩猟</t>
   </si>
   <si>
     <t>沼地酔夢譚</t>
   </si>
   <si>
+    <t>늪지취몽담</t>
+  </si>
+  <si>
     <t>21900z</t>
   </si>
   <si>
+    <t>돌고 모여서 회귀하리라</t>
+  </si>
+  <si>
     <t>シャガルマガラの討伐</t>
   </si>
   <si>
@@ -3226,6 +3436,9 @@
     <t>獄炎に座す、覇たる者</t>
   </si>
   <si>
+    <t>옥염에 앉은, 패자되는 자</t>
+  </si>
+  <si>
     <t>アカムトルムの討伐</t>
   </si>
   <si>
@@ -3233,6 +3446,9 @@
   </si>
   <si>
     <t>無理した弟子の、後始末</t>
+  </si>
+  <si>
+    <t>무리해버린 제자의, 뒤처리</t>
   </si>
   <si>
     <t>ブラキディオスの頭部破壊</t>
@@ -3614,14 +3830,14 @@
   <dimension ref="A1:J340"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="1" topLeftCell="C248" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G264" sqref="G264"/>
+      <pane ySplit="1" topLeftCell="A327" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B340" sqref="B340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.140625" customWidth="1"/>
+    <col min="2" max="2" width="67" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -12116,26 +12332,29 @@
       <c r="A266" t="s">
         <v>857</v>
       </c>
+      <c r="B266" t="s">
+        <v>858</v>
+      </c>
       <c r="C266" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D266" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="E266" t="s">
         <v>14</v>
       </c>
       <c r="F266" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="G266" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="H266" t="s">
         <v>681</v>
       </c>
       <c r="I266" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="J266" t="s">
         <v>67</v>
@@ -12143,19 +12362,22 @@
     </row>
     <row r="267" spans="1:10">
       <c r="A267" t="s">
-        <v>863</v>
+        <v>864</v>
+      </c>
+      <c r="B267" t="s">
+        <v>865</v>
       </c>
       <c r="C267" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D267" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="E267" t="s">
         <v>14</v>
       </c>
       <c r="F267" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="G267" t="s">
         <v>24</v>
@@ -12172,28 +12394,31 @@
     </row>
     <row r="268" spans="1:10">
       <c r="A268" t="s">
+        <v>868</v>
+      </c>
+      <c r="B268" t="s">
+        <v>869</v>
+      </c>
+      <c r="C268" t="s">
+        <v>859</v>
+      </c>
+      <c r="D268" t="s">
         <v>866</v>
       </c>
-      <c r="C268" t="s">
-        <v>858</v>
-      </c>
-      <c r="D268" t="s">
-        <v>864</v>
-      </c>
       <c r="E268" t="s">
         <v>14</v>
       </c>
       <c r="F268" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="G268" t="s">
         <v>24</v>
       </c>
       <c r="H268" t="s">
-        <v>867</v>
+        <v>870</v>
       </c>
       <c r="I268" t="s">
-        <v>868</v>
+        <v>871</v>
       </c>
       <c r="J268" t="s">
         <v>25</v>
@@ -12201,22 +12426,25 @@
     </row>
     <row r="269" spans="1:10">
       <c r="A269" t="s">
-        <v>869</v>
+        <v>872</v>
+      </c>
+      <c r="B269" t="s">
+        <v>873</v>
       </c>
       <c r="C269" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D269" t="s">
-        <v>870</v>
+        <v>874</v>
       </c>
       <c r="E269" t="s">
         <v>14</v>
       </c>
       <c r="F269" t="s">
-        <v>871</v>
+        <v>875</v>
       </c>
       <c r="G269" t="s">
-        <v>872</v>
+        <v>876</v>
       </c>
       <c r="H269" t="s">
         <v>333</v>
@@ -12230,22 +12458,25 @@
     </row>
     <row r="270" spans="1:10">
       <c r="A270" t="s">
-        <v>873</v>
+        <v>877</v>
+      </c>
+      <c r="B270" t="s">
+        <v>878</v>
       </c>
       <c r="C270" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D270" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="E270" t="s">
         <v>14</v>
       </c>
       <c r="F270" t="s">
-        <v>875</v>
+        <v>880</v>
       </c>
       <c r="G270" t="s">
-        <v>876</v>
+        <v>881</v>
       </c>
       <c r="H270" t="s">
         <v>48</v>
@@ -12259,28 +12490,31 @@
     </row>
     <row r="271" spans="1:10">
       <c r="A271" t="s">
-        <v>877</v>
+        <v>882</v>
+      </c>
+      <c r="B271" t="s">
+        <v>883</v>
       </c>
       <c r="C271" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D271" t="s">
-        <v>878</v>
+        <v>884</v>
       </c>
       <c r="E271" t="s">
         <v>14</v>
       </c>
       <c r="F271" t="s">
-        <v>879</v>
+        <v>885</v>
       </c>
       <c r="G271" t="s">
         <v>24</v>
       </c>
       <c r="H271" t="s">
-        <v>880</v>
+        <v>886</v>
       </c>
       <c r="I271" t="s">
-        <v>881</v>
+        <v>887</v>
       </c>
       <c r="J271" t="s">
         <v>25</v>
@@ -12288,19 +12522,22 @@
     </row>
     <row r="272" spans="1:10">
       <c r="A272" t="s">
-        <v>882</v>
+        <v>888</v>
+      </c>
+      <c r="B272" t="s">
+        <v>889</v>
       </c>
       <c r="C272" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D272" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="E272" t="s">
         <v>14</v>
       </c>
       <c r="F272" t="s">
-        <v>883</v>
+        <v>890</v>
       </c>
       <c r="G272" t="s">
         <v>24</v>
@@ -12309,7 +12546,7 @@
         <v>53</v>
       </c>
       <c r="I272" t="s">
-        <v>884</v>
+        <v>891</v>
       </c>
       <c r="J272" t="s">
         <v>25</v>
@@ -12317,28 +12554,31 @@
     </row>
     <row r="273" spans="1:10">
       <c r="A273" t="s">
-        <v>885</v>
+        <v>892</v>
+      </c>
+      <c r="B273" t="s">
+        <v>893</v>
       </c>
       <c r="C273" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D273" t="s">
-        <v>878</v>
+        <v>884</v>
       </c>
       <c r="E273" t="s">
         <v>14</v>
       </c>
       <c r="F273" t="s">
-        <v>886</v>
+        <v>894</v>
       </c>
       <c r="G273" t="s">
-        <v>887</v>
+        <v>895</v>
       </c>
       <c r="H273" t="s">
         <v>53</v>
       </c>
       <c r="I273" t="s">
-        <v>884</v>
+        <v>891</v>
       </c>
       <c r="J273" t="s">
         <v>75</v>
@@ -12346,22 +12586,25 @@
     </row>
     <row r="274" spans="1:10">
       <c r="A274" t="s">
-        <v>888</v>
+        <v>896</v>
+      </c>
+      <c r="B274" t="s">
+        <v>897</v>
       </c>
       <c r="C274" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D274" t="s">
-        <v>889</v>
+        <v>898</v>
       </c>
       <c r="E274" t="s">
         <v>14</v>
       </c>
       <c r="F274" t="s">
-        <v>890</v>
+        <v>899</v>
       </c>
       <c r="G274" t="s">
-        <v>891</v>
+        <v>900</v>
       </c>
       <c r="H274" t="s">
         <v>48</v>
@@ -12375,19 +12618,22 @@
     </row>
     <row r="275" spans="1:10">
       <c r="A275" t="s">
-        <v>892</v>
+        <v>901</v>
+      </c>
+      <c r="B275" t="s">
+        <v>902</v>
       </c>
       <c r="C275" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D275" t="s">
-        <v>893</v>
+        <v>903</v>
       </c>
       <c r="E275" t="s">
         <v>14</v>
       </c>
       <c r="F275" t="s">
-        <v>894</v>
+        <v>904</v>
       </c>
       <c r="G275" t="s">
         <v>24</v>
@@ -12396,7 +12642,7 @@
         <v>681</v>
       </c>
       <c r="I275" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="J275" t="s">
         <v>25</v>
@@ -12404,28 +12650,31 @@
     </row>
     <row r="276" spans="1:10">
       <c r="A276" t="s">
-        <v>895</v>
+        <v>905</v>
+      </c>
+      <c r="B276" t="s">
+        <v>906</v>
       </c>
       <c r="C276" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D276" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="E276" t="s">
         <v>14</v>
       </c>
       <c r="F276" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="G276" t="s">
-        <v>896</v>
+        <v>907</v>
       </c>
       <c r="H276" t="s">
         <v>18</v>
       </c>
       <c r="I276" t="s">
-        <v>897</v>
+        <v>908</v>
       </c>
       <c r="J276" t="s">
         <v>75</v>
@@ -12435,26 +12684,29 @@
       <c r="A277" t="s">
         <v>328</v>
       </c>
+      <c r="B277" t="s">
+        <v>329</v>
+      </c>
       <c r="C277" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D277" t="s">
-        <v>889</v>
+        <v>898</v>
       </c>
       <c r="E277" t="s">
         <v>330</v>
       </c>
       <c r="F277" t="s">
-        <v>898</v>
+        <v>909</v>
       </c>
       <c r="G277" t="s">
-        <v>899</v>
+        <v>910</v>
       </c>
       <c r="H277" t="s">
         <v>53</v>
       </c>
       <c r="I277" t="s">
-        <v>884</v>
+        <v>891</v>
       </c>
       <c r="J277" t="s">
         <v>91</v>
@@ -12464,26 +12716,29 @@
       <c r="A278" t="s">
         <v>352</v>
       </c>
+      <c r="B278" t="s">
+        <v>353</v>
+      </c>
       <c r="C278" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D278" t="s">
-        <v>900</v>
+        <v>911</v>
       </c>
       <c r="E278" t="s">
         <v>330</v>
       </c>
       <c r="F278" t="s">
-        <v>901</v>
+        <v>912</v>
       </c>
       <c r="G278" t="s">
-        <v>902</v>
+        <v>913</v>
       </c>
       <c r="H278" t="s">
         <v>53</v>
       </c>
       <c r="I278" t="s">
-        <v>884</v>
+        <v>891</v>
       </c>
       <c r="J278" t="s">
         <v>91</v>
@@ -12491,28 +12746,31 @@
     </row>
     <row r="279" spans="1:10">
       <c r="A279" t="s">
-        <v>903</v>
+        <v>914</v>
+      </c>
+      <c r="B279" t="s">
+        <v>915</v>
       </c>
       <c r="C279" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D279" t="s">
-        <v>878</v>
+        <v>884</v>
       </c>
       <c r="E279" t="s">
         <v>14</v>
       </c>
       <c r="F279" t="s">
-        <v>904</v>
+        <v>916</v>
       </c>
       <c r="G279" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="H279" t="s">
         <v>67</v>
       </c>
       <c r="I279" t="s">
-        <v>905</v>
+        <v>917</v>
       </c>
       <c r="J279" t="s">
         <v>67</v>
@@ -12520,19 +12778,22 @@
     </row>
     <row r="280" spans="1:10">
       <c r="A280" t="s">
-        <v>906</v>
+        <v>918</v>
+      </c>
+      <c r="B280" t="s">
+        <v>919</v>
       </c>
       <c r="C280" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D280" t="s">
-        <v>870</v>
+        <v>874</v>
       </c>
       <c r="E280" t="s">
         <v>14</v>
       </c>
       <c r="F280" t="s">
-        <v>907</v>
+        <v>920</v>
       </c>
       <c r="G280" t="s">
         <v>24</v>
@@ -12549,22 +12810,25 @@
     </row>
     <row r="281" spans="1:10">
       <c r="A281" t="s">
-        <v>908</v>
+        <v>921</v>
+      </c>
+      <c r="B281" t="s">
+        <v>922</v>
       </c>
       <c r="C281" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D281" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="E281" t="s">
         <v>14</v>
       </c>
       <c r="F281" t="s">
-        <v>909</v>
+        <v>923</v>
       </c>
       <c r="G281" t="s">
-        <v>910</v>
+        <v>924</v>
       </c>
       <c r="H281" t="s">
         <v>548</v>
@@ -12578,22 +12842,25 @@
     </row>
     <row r="282" spans="1:10">
       <c r="A282" t="s">
-        <v>911</v>
+        <v>925</v>
+      </c>
+      <c r="B282" t="s">
+        <v>926</v>
       </c>
       <c r="C282" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D282" t="s">
-        <v>870</v>
+        <v>874</v>
       </c>
       <c r="E282" t="s">
         <v>14</v>
       </c>
       <c r="F282" t="s">
-        <v>912</v>
+        <v>927</v>
       </c>
       <c r="G282" t="s">
-        <v>913</v>
+        <v>928</v>
       </c>
       <c r="H282" t="s">
         <v>48</v>
@@ -12607,28 +12874,31 @@
     </row>
     <row r="283" spans="1:10">
       <c r="A283" t="s">
-        <v>914</v>
+        <v>929</v>
+      </c>
+      <c r="B283" t="s">
+        <v>930</v>
       </c>
       <c r="C283" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D283" t="s">
-        <v>915</v>
+        <v>931</v>
       </c>
       <c r="E283" t="s">
         <v>14</v>
       </c>
       <c r="F283" t="s">
-        <v>916</v>
+        <v>932</v>
       </c>
       <c r="G283" t="s">
-        <v>917</v>
+        <v>933</v>
       </c>
       <c r="H283" t="s">
         <v>681</v>
       </c>
       <c r="I283" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="J283" t="s">
         <v>75</v>
@@ -12636,28 +12906,31 @@
     </row>
     <row r="284" spans="1:10">
       <c r="A284" t="s">
-        <v>918</v>
+        <v>934</v>
+      </c>
+      <c r="B284" t="s">
+        <v>935</v>
       </c>
       <c r="C284" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D284" t="s">
-        <v>919</v>
+        <v>936</v>
       </c>
       <c r="E284" t="s">
         <v>14</v>
       </c>
       <c r="F284" t="s">
-        <v>920</v>
+        <v>937</v>
       </c>
       <c r="G284" t="s">
-        <v>921</v>
+        <v>938</v>
       </c>
       <c r="H284" t="s">
-        <v>922</v>
+        <v>939</v>
       </c>
       <c r="I284" t="s">
-        <v>923</v>
+        <v>940</v>
       </c>
       <c r="J284" t="s">
         <v>91</v>
@@ -12665,22 +12938,25 @@
     </row>
     <row r="285" spans="1:10">
       <c r="A285" t="s">
-        <v>924</v>
+        <v>941</v>
+      </c>
+      <c r="B285" t="s">
+        <v>942</v>
       </c>
       <c r="C285" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D285" t="s">
-        <v>925</v>
+        <v>943</v>
       </c>
       <c r="E285" t="s">
         <v>14</v>
       </c>
       <c r="F285" t="s">
-        <v>926</v>
+        <v>944</v>
       </c>
       <c r="G285" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="H285" t="s">
         <v>618</v>
@@ -12694,22 +12970,25 @@
     </row>
     <row r="286" spans="1:10">
       <c r="A286" t="s">
-        <v>927</v>
+        <v>945</v>
+      </c>
+      <c r="B286" t="s">
+        <v>946</v>
       </c>
       <c r="C286" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D286" t="s">
-        <v>870</v>
+        <v>874</v>
       </c>
       <c r="E286" t="s">
         <v>14</v>
       </c>
       <c r="F286" t="s">
-        <v>928</v>
+        <v>947</v>
       </c>
       <c r="G286" t="s">
-        <v>929</v>
+        <v>948</v>
       </c>
       <c r="H286" t="s">
         <v>691</v>
@@ -12723,28 +13002,31 @@
     </row>
     <row r="287" spans="1:10">
       <c r="A287" t="s">
-        <v>930</v>
+        <v>949</v>
+      </c>
+      <c r="B287" t="s">
+        <v>950</v>
       </c>
       <c r="C287" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D287" t="s">
-        <v>870</v>
+        <v>874</v>
       </c>
       <c r="E287" t="s">
         <v>14</v>
       </c>
       <c r="F287" t="s">
-        <v>931</v>
+        <v>951</v>
       </c>
       <c r="G287" t="s">
-        <v>932</v>
+        <v>952</v>
       </c>
       <c r="H287" t="s">
         <v>681</v>
       </c>
       <c r="I287" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="J287" t="s">
         <v>75</v>
@@ -12752,22 +13034,25 @@
     </row>
     <row r="288" spans="1:10">
       <c r="A288" t="s">
-        <v>933</v>
+        <v>953</v>
+      </c>
+      <c r="B288" t="s">
+        <v>954</v>
       </c>
       <c r="C288" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D288" t="s">
-        <v>900</v>
+        <v>911</v>
       </c>
       <c r="E288" t="s">
         <v>14</v>
       </c>
       <c r="F288" t="s">
-        <v>934</v>
+        <v>955</v>
       </c>
       <c r="G288" t="s">
-        <v>935</v>
+        <v>956</v>
       </c>
       <c r="H288" t="s">
         <v>48</v>
@@ -12781,22 +13066,25 @@
     </row>
     <row r="289" spans="1:10">
       <c r="A289" t="s">
-        <v>936</v>
+        <v>957</v>
+      </c>
+      <c r="B289" t="s">
+        <v>958</v>
       </c>
       <c r="C289" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D289" t="s">
-        <v>915</v>
+        <v>931</v>
       </c>
       <c r="E289" t="s">
         <v>14</v>
       </c>
       <c r="F289" t="s">
-        <v>937</v>
+        <v>959</v>
       </c>
       <c r="G289" t="s">
-        <v>938</v>
+        <v>960</v>
       </c>
       <c r="H289" t="s">
         <v>618</v>
@@ -12810,19 +13098,22 @@
     </row>
     <row r="290" spans="1:10">
       <c r="A290" t="s">
-        <v>939</v>
+        <v>961</v>
+      </c>
+      <c r="B290" t="s">
+        <v>962</v>
       </c>
       <c r="C290" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D290" t="s">
-        <v>915</v>
+        <v>931</v>
       </c>
       <c r="E290" t="s">
         <v>14</v>
       </c>
       <c r="F290" t="s">
-        <v>940</v>
+        <v>963</v>
       </c>
       <c r="G290" t="s">
         <v>24</v>
@@ -12831,7 +13122,7 @@
         <v>91</v>
       </c>
       <c r="I290" t="s">
-        <v>941</v>
+        <v>964</v>
       </c>
       <c r="J290" t="s">
         <v>25</v>
@@ -12839,19 +13130,22 @@
     </row>
     <row r="291" spans="1:10">
       <c r="A291" t="s">
-        <v>942</v>
+        <v>965</v>
+      </c>
+      <c r="B291" t="s">
+        <v>966</v>
       </c>
       <c r="C291" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D291" t="s">
-        <v>943</v>
+        <v>967</v>
       </c>
       <c r="E291" t="s">
         <v>14</v>
       </c>
       <c r="F291" t="s">
-        <v>944</v>
+        <v>968</v>
       </c>
       <c r="G291" t="s">
         <v>24</v>
@@ -12860,7 +13154,7 @@
         <v>91</v>
       </c>
       <c r="I291" t="s">
-        <v>941</v>
+        <v>964</v>
       </c>
       <c r="J291" t="s">
         <v>25</v>
@@ -12868,28 +13162,31 @@
     </row>
     <row r="292" spans="1:10">
       <c r="A292" t="s">
-        <v>945</v>
+        <v>969</v>
+      </c>
+      <c r="B292" t="s">
+        <v>970</v>
       </c>
       <c r="C292" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D292" t="s">
-        <v>946</v>
+        <v>971</v>
       </c>
       <c r="E292" t="s">
         <v>14</v>
       </c>
       <c r="F292" t="s">
-        <v>947</v>
+        <v>972</v>
       </c>
       <c r="G292" t="s">
-        <v>948</v>
+        <v>973</v>
       </c>
       <c r="H292" t="s">
         <v>681</v>
       </c>
       <c r="I292" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="J292" t="s">
         <v>75</v>
@@ -12897,28 +13194,31 @@
     </row>
     <row r="293" spans="1:10">
       <c r="A293" t="s">
-        <v>949</v>
+        <v>974</v>
+      </c>
+      <c r="B293" t="s">
+        <v>975</v>
       </c>
       <c r="C293" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D293" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="E293" t="s">
         <v>14</v>
       </c>
       <c r="F293" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="G293" t="s">
-        <v>896</v>
+        <v>907</v>
       </c>
       <c r="H293" t="s">
         <v>53</v>
       </c>
       <c r="I293" t="s">
-        <v>950</v>
+        <v>976</v>
       </c>
       <c r="J293" t="s">
         <v>75</v>
@@ -12926,28 +13226,31 @@
     </row>
     <row r="294" spans="1:10">
       <c r="A294" t="s">
-        <v>951</v>
+        <v>977</v>
+      </c>
+      <c r="B294" t="s">
+        <v>978</v>
       </c>
       <c r="C294" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D294" t="s">
-        <v>915</v>
+        <v>931</v>
       </c>
       <c r="E294" t="s">
         <v>14</v>
       </c>
       <c r="F294" t="s">
-        <v>886</v>
+        <v>894</v>
       </c>
       <c r="G294" t="s">
-        <v>887</v>
+        <v>895</v>
       </c>
       <c r="H294" t="s">
         <v>53</v>
       </c>
       <c r="I294" t="s">
-        <v>884</v>
+        <v>891</v>
       </c>
       <c r="J294" t="s">
         <v>91</v>
@@ -12955,19 +13258,22 @@
     </row>
     <row r="295" spans="1:10">
       <c r="A295" t="s">
-        <v>952</v>
+        <v>979</v>
+      </c>
+      <c r="B295" t="s">
+        <v>980</v>
       </c>
       <c r="C295" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D295" t="s">
-        <v>946</v>
+        <v>971</v>
       </c>
       <c r="E295" t="s">
         <v>14</v>
       </c>
       <c r="F295" t="s">
-        <v>953</v>
+        <v>981</v>
       </c>
       <c r="G295" t="s">
         <v>24</v>
@@ -12984,19 +13290,22 @@
     </row>
     <row r="296" spans="1:10">
       <c r="A296" t="s">
-        <v>954</v>
+        <v>982</v>
+      </c>
+      <c r="B296" t="s">
+        <v>983</v>
       </c>
       <c r="C296" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D296" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="E296" t="s">
         <v>14</v>
       </c>
       <c r="F296" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="G296" t="s">
         <v>24</v>
@@ -13005,7 +13314,7 @@
         <v>451</v>
       </c>
       <c r="I296" t="s">
-        <v>955</v>
+        <v>984</v>
       </c>
       <c r="J296" t="s">
         <v>25</v>
@@ -13013,22 +13322,25 @@
     </row>
     <row r="297" spans="1:10">
       <c r="A297" t="s">
-        <v>956</v>
+        <v>985</v>
+      </c>
+      <c r="B297" t="s">
+        <v>986</v>
       </c>
       <c r="C297" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D297" t="s">
-        <v>957</v>
+        <v>987</v>
       </c>
       <c r="E297" t="s">
         <v>14</v>
       </c>
       <c r="F297" t="s">
-        <v>958</v>
+        <v>988</v>
       </c>
       <c r="G297" t="s">
-        <v>959</v>
+        <v>989</v>
       </c>
       <c r="H297" t="s">
         <v>618</v>
@@ -13042,22 +13354,25 @@
     </row>
     <row r="298" spans="1:10">
       <c r="A298" t="s">
-        <v>960</v>
+        <v>990</v>
+      </c>
+      <c r="B298" t="s">
+        <v>991</v>
       </c>
       <c r="C298" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D298" t="s">
-        <v>961</v>
+        <v>992</v>
       </c>
       <c r="E298" t="s">
         <v>14</v>
       </c>
       <c r="F298" t="s">
-        <v>962</v>
+        <v>993</v>
       </c>
       <c r="G298" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="H298" t="s">
         <v>548</v>
@@ -13071,28 +13386,31 @@
     </row>
     <row r="299" spans="1:10">
       <c r="A299" t="s">
-        <v>963</v>
+        <v>994</v>
+      </c>
+      <c r="B299" t="s">
+        <v>995</v>
       </c>
       <c r="C299" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D299" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="E299" t="s">
         <v>14</v>
       </c>
       <c r="F299" t="s">
-        <v>964</v>
+        <v>996</v>
       </c>
       <c r="G299" t="s">
-        <v>965</v>
+        <v>997</v>
       </c>
       <c r="H299" t="s">
         <v>681</v>
       </c>
       <c r="I299" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="J299" t="s">
         <v>75</v>
@@ -13100,28 +13418,31 @@
     </row>
     <row r="300" spans="1:10">
       <c r="A300" t="s">
-        <v>966</v>
+        <v>998</v>
+      </c>
+      <c r="B300" t="s">
+        <v>999</v>
       </c>
       <c r="C300" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D300" t="s">
-        <v>925</v>
+        <v>943</v>
       </c>
       <c r="E300" t="s">
         <v>14</v>
       </c>
       <c r="F300" t="s">
-        <v>967</v>
+        <v>1000</v>
       </c>
       <c r="G300" t="s">
-        <v>968</v>
+        <v>1001</v>
       </c>
       <c r="H300" t="s">
         <v>53</v>
       </c>
       <c r="I300" t="s">
-        <v>884</v>
+        <v>891</v>
       </c>
       <c r="J300" t="s">
         <v>75</v>
@@ -13129,28 +13450,31 @@
     </row>
     <row r="301" spans="1:10">
       <c r="A301" t="s">
-        <v>969</v>
+        <v>1002</v>
+      </c>
+      <c r="B301" t="s">
+        <v>1003</v>
       </c>
       <c r="C301" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D301" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="E301" t="s">
         <v>14</v>
       </c>
       <c r="F301" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="G301" t="s">
-        <v>970</v>
+        <v>1004</v>
       </c>
       <c r="H301" t="s">
         <v>647</v>
       </c>
       <c r="I301" t="s">
-        <v>971</v>
+        <v>1005</v>
       </c>
       <c r="J301" t="s">
         <v>75</v>
@@ -13158,28 +13482,31 @@
     </row>
     <row r="302" spans="1:10">
       <c r="A302" t="s">
-        <v>972</v>
+        <v>1006</v>
+      </c>
+      <c r="B302" t="s">
+        <v>1007</v>
       </c>
       <c r="C302" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D302" t="s">
-        <v>878</v>
+        <v>884</v>
       </c>
       <c r="E302" t="s">
         <v>14</v>
       </c>
       <c r="F302" t="s">
-        <v>973</v>
+        <v>1008</v>
       </c>
       <c r="G302" t="s">
-        <v>974</v>
+        <v>1009</v>
       </c>
       <c r="H302" t="s">
-        <v>975</v>
+        <v>1010</v>
       </c>
       <c r="I302" t="s">
-        <v>976</v>
+        <v>1011</v>
       </c>
       <c r="J302" t="s">
         <v>53</v>
@@ -13187,28 +13514,31 @@
     </row>
     <row r="303" spans="1:10">
       <c r="A303" t="s">
-        <v>977</v>
+        <v>1012</v>
+      </c>
+      <c r="B303" t="s">
+        <v>1013</v>
       </c>
       <c r="C303" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D303" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="E303" t="s">
         <v>330</v>
       </c>
       <c r="F303" t="s">
-        <v>978</v>
+        <v>1014</v>
       </c>
       <c r="G303" t="s">
-        <v>979</v>
+        <v>1015</v>
       </c>
       <c r="H303" t="s">
         <v>53</v>
       </c>
       <c r="I303" t="s">
-        <v>884</v>
+        <v>891</v>
       </c>
       <c r="J303" t="s">
         <v>91</v>
@@ -13216,28 +13546,31 @@
     </row>
     <row r="304" spans="1:10">
       <c r="A304" t="s">
-        <v>980</v>
+        <v>1016</v>
+      </c>
+      <c r="B304" t="s">
+        <v>1017</v>
       </c>
       <c r="C304" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D304" t="s">
-        <v>981</v>
+        <v>1018</v>
       </c>
       <c r="E304" t="s">
         <v>14</v>
       </c>
       <c r="F304" t="s">
-        <v>982</v>
+        <v>1019</v>
       </c>
       <c r="G304" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="H304" t="s">
         <v>618</v>
       </c>
       <c r="I304" t="s">
-        <v>983</v>
+        <v>1020</v>
       </c>
       <c r="J304" t="s">
         <v>67</v>
@@ -13245,22 +13578,25 @@
     </row>
     <row r="305" spans="1:10">
       <c r="A305" t="s">
-        <v>984</v>
+        <v>1021</v>
+      </c>
+      <c r="B305" t="s">
+        <v>1022</v>
       </c>
       <c r="C305" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D305" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="E305" t="s">
         <v>14</v>
       </c>
       <c r="F305" t="s">
-        <v>964</v>
+        <v>996</v>
       </c>
       <c r="G305" t="s">
-        <v>985</v>
+        <v>1023</v>
       </c>
       <c r="H305" t="s">
         <v>333</v>
@@ -13274,28 +13610,31 @@
     </row>
     <row r="306" spans="1:10">
       <c r="A306" t="s">
-        <v>986</v>
+        <v>1024</v>
+      </c>
+      <c r="B306" t="s">
+        <v>1025</v>
       </c>
       <c r="C306" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D306" t="s">
-        <v>987</v>
+        <v>1026</v>
       </c>
       <c r="E306" t="s">
         <v>14</v>
       </c>
       <c r="F306" t="s">
-        <v>988</v>
+        <v>1027</v>
       </c>
       <c r="G306" t="s">
-        <v>989</v>
+        <v>1028</v>
       </c>
       <c r="H306" t="s">
-        <v>922</v>
+        <v>939</v>
       </c>
       <c r="I306" t="s">
-        <v>923</v>
+        <v>940</v>
       </c>
       <c r="J306" t="s">
         <v>91</v>
@@ -13303,28 +13642,31 @@
     </row>
     <row r="307" spans="1:10">
       <c r="A307" t="s">
-        <v>990</v>
+        <v>1029</v>
+      </c>
+      <c r="B307" t="s">
+        <v>1030</v>
       </c>
       <c r="C307" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D307" t="s">
-        <v>878</v>
+        <v>884</v>
       </c>
       <c r="E307" t="s">
         <v>14</v>
       </c>
       <c r="F307" t="s">
-        <v>991</v>
+        <v>1031</v>
       </c>
       <c r="G307" t="s">
-        <v>992</v>
+        <v>1032</v>
       </c>
       <c r="H307" t="s">
-        <v>975</v>
+        <v>1010</v>
       </c>
       <c r="I307" t="s">
-        <v>993</v>
+        <v>1033</v>
       </c>
       <c r="J307" t="s">
         <v>75</v>
@@ -13332,28 +13674,31 @@
     </row>
     <row r="308" spans="1:10">
       <c r="A308" t="s">
-        <v>994</v>
+        <v>1034</v>
+      </c>
+      <c r="B308" t="s">
+        <v>1035</v>
       </c>
       <c r="C308" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D308" t="s">
-        <v>946</v>
+        <v>971</v>
       </c>
       <c r="E308" t="s">
         <v>330</v>
       </c>
       <c r="F308" t="s">
-        <v>898</v>
+        <v>909</v>
       </c>
       <c r="G308" t="s">
-        <v>995</v>
+        <v>1036</v>
       </c>
       <c r="H308" t="s">
         <v>53</v>
       </c>
       <c r="I308" t="s">
-        <v>884</v>
+        <v>891</v>
       </c>
       <c r="J308" t="s">
         <v>91</v>
@@ -13361,22 +13706,25 @@
     </row>
     <row r="309" spans="1:10">
       <c r="A309" t="s">
-        <v>996</v>
+        <v>1037</v>
+      </c>
+      <c r="B309" t="s">
+        <v>1038</v>
       </c>
       <c r="C309" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D309" t="s">
-        <v>900</v>
+        <v>911</v>
       </c>
       <c r="E309" t="s">
         <v>14</v>
       </c>
       <c r="F309" t="s">
-        <v>991</v>
+        <v>1031</v>
       </c>
       <c r="G309" t="s">
-        <v>997</v>
+        <v>1039</v>
       </c>
       <c r="H309" t="s">
         <v>691</v>
@@ -13390,19 +13738,22 @@
     </row>
     <row r="310" spans="1:10">
       <c r="A310" t="s">
-        <v>998</v>
+        <v>1040</v>
+      </c>
+      <c r="B310" t="s">
+        <v>1041</v>
       </c>
       <c r="C310" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D310" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="E310" t="s">
         <v>14</v>
       </c>
       <c r="F310" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="G310" t="s">
         <v>24</v>
@@ -13419,22 +13770,25 @@
     </row>
     <row r="311" spans="1:10">
       <c r="A311" t="s">
-        <v>999</v>
+        <v>1042</v>
+      </c>
+      <c r="B311" t="s">
+        <v>1043</v>
       </c>
       <c r="C311" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D311" t="s">
-        <v>878</v>
+        <v>884</v>
       </c>
       <c r="E311" t="s">
         <v>14</v>
       </c>
       <c r="F311" t="s">
-        <v>1000</v>
+        <v>1044</v>
       </c>
       <c r="G311" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="H311" t="s">
         <v>548</v>
@@ -13448,28 +13802,31 @@
     </row>
     <row r="312" spans="1:10">
       <c r="A312" t="s">
-        <v>1001</v>
+        <v>1045</v>
+      </c>
+      <c r="B312" t="s">
+        <v>1046</v>
       </c>
       <c r="C312" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D312" t="s">
-        <v>900</v>
+        <v>911</v>
       </c>
       <c r="E312" t="s">
         <v>14</v>
       </c>
       <c r="F312" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="G312" t="s">
-        <v>1002</v>
+        <v>1047</v>
       </c>
       <c r="H312" t="s">
         <v>53</v>
       </c>
       <c r="I312" t="s">
-        <v>1003</v>
+        <v>1048</v>
       </c>
       <c r="J312" t="s">
         <v>369</v>
@@ -13477,28 +13834,31 @@
     </row>
     <row r="313" spans="1:10">
       <c r="A313" t="s">
-        <v>1004</v>
+        <v>1049</v>
+      </c>
+      <c r="B313" t="s">
+        <v>1050</v>
       </c>
       <c r="C313" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D313" t="s">
-        <v>925</v>
+        <v>943</v>
       </c>
       <c r="E313" t="s">
         <v>14</v>
       </c>
       <c r="F313" t="s">
-        <v>1005</v>
+        <v>1051</v>
       </c>
       <c r="G313" t="s">
-        <v>1006</v>
+        <v>1052</v>
       </c>
       <c r="H313" t="s">
         <v>48</v>
       </c>
       <c r="I313" t="s">
-        <v>1007</v>
+        <v>1053</v>
       </c>
       <c r="J313" t="s">
         <v>75</v>
@@ -13506,22 +13866,25 @@
     </row>
     <row r="314" spans="1:10">
       <c r="A314" t="s">
-        <v>1008</v>
+        <v>1054</v>
+      </c>
+      <c r="B314" t="s">
+        <v>1055</v>
       </c>
       <c r="C314" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D314" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="E314" t="s">
         <v>14</v>
       </c>
       <c r="F314" t="s">
-        <v>1009</v>
+        <v>1056</v>
       </c>
       <c r="G314" t="s">
-        <v>1010</v>
+        <v>1057</v>
       </c>
       <c r="H314" t="s">
         <v>333</v>
@@ -13535,19 +13898,22 @@
     </row>
     <row r="315" spans="1:10">
       <c r="A315" t="s">
-        <v>1011</v>
+        <v>1058</v>
+      </c>
+      <c r="B315" t="s">
+        <v>1059</v>
       </c>
       <c r="C315" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D315" t="s">
-        <v>878</v>
+        <v>884</v>
       </c>
       <c r="E315" t="s">
         <v>14</v>
       </c>
       <c r="F315" t="s">
-        <v>1012</v>
+        <v>1060</v>
       </c>
       <c r="G315" t="s">
         <v>24</v>
@@ -13564,28 +13930,31 @@
     </row>
     <row r="316" spans="1:10">
       <c r="A316" t="s">
-        <v>1013</v>
+        <v>1061</v>
+      </c>
+      <c r="B316" t="s">
+        <v>1062</v>
       </c>
       <c r="C316" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D316" t="s">
-        <v>1014</v>
+        <v>1063</v>
       </c>
       <c r="E316" t="s">
         <v>14</v>
       </c>
       <c r="F316" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="G316" t="s">
-        <v>896</v>
+        <v>907</v>
       </c>
       <c r="H316" t="s">
-        <v>1015</v>
+        <v>1064</v>
       </c>
       <c r="I316" t="s">
-        <v>1016</v>
+        <v>1065</v>
       </c>
       <c r="J316" t="s">
         <v>75</v>
@@ -13593,28 +13962,31 @@
     </row>
     <row r="317" spans="1:10">
       <c r="A317" t="s">
-        <v>1017</v>
+        <v>1066</v>
+      </c>
+      <c r="B317" t="s">
+        <v>1067</v>
       </c>
       <c r="C317" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D317" t="s">
-        <v>1014</v>
+        <v>1063</v>
       </c>
       <c r="E317" t="s">
         <v>14</v>
       </c>
       <c r="F317" t="s">
-        <v>1018</v>
+        <v>1068</v>
       </c>
       <c r="G317" t="s">
         <v>24</v>
       </c>
       <c r="H317" t="s">
-        <v>880</v>
+        <v>886</v>
       </c>
       <c r="I317" t="s">
-        <v>881</v>
+        <v>887</v>
       </c>
       <c r="J317" t="s">
         <v>25</v>
@@ -13622,28 +13994,31 @@
     </row>
     <row r="318" spans="1:10">
       <c r="A318" t="s">
-        <v>1019</v>
+        <v>1069</v>
+      </c>
+      <c r="B318" t="s">
+        <v>1070</v>
       </c>
       <c r="C318" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D318" t="s">
-        <v>981</v>
+        <v>1018</v>
       </c>
       <c r="E318" t="s">
         <v>14</v>
       </c>
       <c r="F318" t="s">
-        <v>1018</v>
+        <v>1068</v>
       </c>
       <c r="G318" t="s">
-        <v>896</v>
+        <v>907</v>
       </c>
       <c r="H318" t="s">
         <v>91</v>
       </c>
       <c r="I318" t="s">
-        <v>1020</v>
+        <v>1071</v>
       </c>
       <c r="J318" t="s">
         <v>75</v>
@@ -13651,22 +14026,25 @@
     </row>
     <row r="319" spans="1:10">
       <c r="A319" t="s">
-        <v>1021</v>
+        <v>1072</v>
+      </c>
+      <c r="B319" t="s">
+        <v>1073</v>
       </c>
       <c r="C319" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D319" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="E319" t="s">
         <v>14</v>
       </c>
       <c r="F319" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="G319" t="s">
-        <v>896</v>
+        <v>907</v>
       </c>
       <c r="H319" t="s">
         <v>91</v>
@@ -13680,22 +14058,25 @@
     </row>
     <row r="320" spans="1:10">
       <c r="A320" t="s">
-        <v>1022</v>
+        <v>1074</v>
+      </c>
+      <c r="B320" t="s">
+        <v>1075</v>
       </c>
       <c r="C320" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D320" t="s">
-        <v>878</v>
+        <v>884</v>
       </c>
       <c r="E320" t="s">
         <v>14</v>
       </c>
       <c r="F320" t="s">
-        <v>1023</v>
+        <v>1076</v>
       </c>
       <c r="G320" t="s">
-        <v>1024</v>
+        <v>1077</v>
       </c>
       <c r="H320" t="s">
         <v>333</v>
@@ -13709,28 +14090,31 @@
     </row>
     <row r="321" spans="1:10">
       <c r="A321" t="s">
-        <v>1025</v>
+        <v>1078</v>
+      </c>
+      <c r="B321" t="s">
+        <v>1079</v>
       </c>
       <c r="C321" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D321" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="E321" t="s">
         <v>14</v>
       </c>
       <c r="F321" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="G321" t="s">
-        <v>896</v>
+        <v>907</v>
       </c>
       <c r="H321" t="s">
-        <v>1026</v>
+        <v>1080</v>
       </c>
       <c r="I321" t="s">
-        <v>1027</v>
+        <v>1081</v>
       </c>
       <c r="J321" t="s">
         <v>75</v>
@@ -13740,26 +14124,29 @@
       <c r="A322" t="s">
         <v>389</v>
       </c>
+      <c r="B322" t="s">
+        <v>390</v>
+      </c>
       <c r="C322" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D322" t="s">
-        <v>915</v>
+        <v>931</v>
       </c>
       <c r="E322" t="s">
         <v>330</v>
       </c>
       <c r="F322" t="s">
-        <v>978</v>
+        <v>1014</v>
       </c>
       <c r="G322" t="s">
-        <v>1028</v>
+        <v>1082</v>
       </c>
       <c r="H322" t="s">
         <v>53</v>
       </c>
       <c r="I322" t="s">
-        <v>884</v>
+        <v>891</v>
       </c>
       <c r="J322" t="s">
         <v>91</v>
@@ -13767,28 +14154,31 @@
     </row>
     <row r="323" spans="1:10">
       <c r="A323" t="s">
-        <v>1029</v>
+        <v>1083</v>
+      </c>
+      <c r="B323" t="s">
+        <v>1084</v>
       </c>
       <c r="C323" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D323" t="s">
-        <v>946</v>
+        <v>971</v>
       </c>
       <c r="E323" t="s">
         <v>14</v>
       </c>
       <c r="F323" t="s">
-        <v>1030</v>
+        <v>1085</v>
       </c>
       <c r="G323" t="s">
-        <v>1031</v>
+        <v>1086</v>
       </c>
       <c r="H323" t="s">
         <v>618</v>
       </c>
       <c r="I323" t="s">
-        <v>983</v>
+        <v>1020</v>
       </c>
       <c r="J323" t="s">
         <v>53</v>
@@ -13796,19 +14186,22 @@
     </row>
     <row r="324" spans="1:10">
       <c r="A324" t="s">
-        <v>1032</v>
+        <v>1087</v>
+      </c>
+      <c r="B324" t="s">
+        <v>1088</v>
       </c>
       <c r="C324" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D324" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="E324" t="s">
         <v>14</v>
       </c>
       <c r="F324" t="s">
-        <v>916</v>
+        <v>932</v>
       </c>
       <c r="G324" t="s">
         <v>24</v>
@@ -13825,28 +14218,31 @@
     </row>
     <row r="325" spans="1:10">
       <c r="A325" t="s">
-        <v>1033</v>
+        <v>1089</v>
+      </c>
+      <c r="B325" t="s">
+        <v>1090</v>
       </c>
       <c r="C325" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D325" t="s">
-        <v>1034</v>
+        <v>1091</v>
       </c>
       <c r="E325" t="s">
         <v>14</v>
       </c>
       <c r="F325" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="G325" t="s">
         <v>24</v>
       </c>
       <c r="H325" t="s">
-        <v>1035</v>
+        <v>1092</v>
       </c>
       <c r="I325" t="s">
-        <v>1036</v>
+        <v>1093</v>
       </c>
       <c r="J325" t="s">
         <v>25</v>
@@ -13854,19 +14250,22 @@
     </row>
     <row r="326" spans="1:10">
       <c r="A326" t="s">
-        <v>1037</v>
+        <v>1094</v>
+      </c>
+      <c r="B326" t="s">
+        <v>1095</v>
       </c>
       <c r="C326" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D326" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="E326" t="s">
         <v>14</v>
       </c>
       <c r="F326" t="s">
-        <v>1038</v>
+        <v>1096</v>
       </c>
       <c r="G326" t="s">
         <v>24</v>
@@ -13883,28 +14282,31 @@
     </row>
     <row r="327" spans="1:10">
       <c r="A327" t="s">
-        <v>1039</v>
+        <v>1097</v>
+      </c>
+      <c r="B327" t="s">
+        <v>1098</v>
       </c>
       <c r="C327" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D327" t="s">
-        <v>961</v>
+        <v>992</v>
       </c>
       <c r="E327" t="s">
         <v>330</v>
       </c>
       <c r="F327" t="s">
-        <v>901</v>
+        <v>912</v>
       </c>
       <c r="G327" t="s">
-        <v>1040</v>
+        <v>1099</v>
       </c>
       <c r="H327" t="s">
         <v>53</v>
       </c>
       <c r="I327" t="s">
-        <v>884</v>
+        <v>891</v>
       </c>
       <c r="J327" t="s">
         <v>91</v>
@@ -13912,19 +14314,22 @@
     </row>
     <row r="328" spans="1:10">
       <c r="A328" t="s">
-        <v>1041</v>
+        <v>1100</v>
+      </c>
+      <c r="B328" t="s">
+        <v>1101</v>
       </c>
       <c r="C328" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D328" t="s">
-        <v>1042</v>
+        <v>1102</v>
       </c>
       <c r="E328" t="s">
         <v>14</v>
       </c>
       <c r="F328" t="s">
-        <v>1043</v>
+        <v>1103</v>
       </c>
       <c r="G328" t="s">
         <v>24</v>
@@ -13941,28 +14346,31 @@
     </row>
     <row r="329" spans="1:10">
       <c r="A329" t="s">
-        <v>1044</v>
+        <v>1104</v>
+      </c>
+      <c r="B329" t="s">
+        <v>1105</v>
       </c>
       <c r="C329" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D329" t="s">
-        <v>1045</v>
+        <v>1106</v>
       </c>
       <c r="E329" t="s">
         <v>14</v>
       </c>
       <c r="F329" t="s">
-        <v>1046</v>
+        <v>1107</v>
       </c>
       <c r="G329" t="s">
-        <v>1047</v>
+        <v>1108</v>
       </c>
       <c r="H329" t="s">
         <v>91</v>
       </c>
       <c r="I329" t="s">
-        <v>941</v>
+        <v>964</v>
       </c>
       <c r="J329" t="s">
         <v>91</v>
@@ -13970,19 +14378,22 @@
     </row>
     <row r="330" spans="1:10">
       <c r="A330" t="s">
-        <v>1048</v>
+        <v>1109</v>
+      </c>
+      <c r="B330" t="s">
+        <v>1110</v>
       </c>
       <c r="C330" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D330" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="E330" t="s">
         <v>14</v>
       </c>
       <c r="F330" t="s">
-        <v>1049</v>
+        <v>1111</v>
       </c>
       <c r="G330" t="s">
         <v>24</v>
@@ -13999,28 +14410,31 @@
     </row>
     <row r="331" spans="1:10">
       <c r="A331" t="s">
-        <v>1050</v>
+        <v>1112</v>
+      </c>
+      <c r="B331" t="s">
+        <v>1113</v>
       </c>
       <c r="C331" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D331" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="E331" t="s">
         <v>14</v>
       </c>
       <c r="F331" t="s">
-        <v>904</v>
+        <v>916</v>
       </c>
       <c r="G331" t="s">
-        <v>1051</v>
+        <v>1114</v>
       </c>
       <c r="H331" t="s">
-        <v>1035</v>
+        <v>1092</v>
       </c>
       <c r="I331" t="s">
-        <v>1052</v>
+        <v>1115</v>
       </c>
       <c r="J331" t="s">
         <v>75</v>
@@ -14028,28 +14442,31 @@
     </row>
     <row r="332" spans="1:10">
       <c r="A332" t="s">
-        <v>1053</v>
+        <v>1116</v>
+      </c>
+      <c r="B332" t="s">
+        <v>1117</v>
       </c>
       <c r="C332" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D332" t="s">
-        <v>870</v>
+        <v>874</v>
       </c>
       <c r="E332" t="s">
         <v>14</v>
       </c>
       <c r="F332" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="G332" t="s">
-        <v>1054</v>
+        <v>1118</v>
       </c>
       <c r="H332" t="s">
-        <v>880</v>
+        <v>886</v>
       </c>
       <c r="I332" t="s">
-        <v>881</v>
+        <v>887</v>
       </c>
       <c r="J332" t="s">
         <v>75</v>
@@ -14057,28 +14474,31 @@
     </row>
     <row r="333" spans="1:10">
       <c r="A333" t="s">
-        <v>1055</v>
+        <v>1119</v>
+      </c>
+      <c r="B333" t="s">
+        <v>1120</v>
       </c>
       <c r="C333" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D333" t="s">
-        <v>957</v>
+        <v>987</v>
       </c>
       <c r="E333" t="s">
         <v>14</v>
       </c>
       <c r="F333" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="G333" t="s">
-        <v>896</v>
+        <v>907</v>
       </c>
       <c r="H333" t="s">
-        <v>1056</v>
+        <v>1121</v>
       </c>
       <c r="I333" t="s">
-        <v>1057</v>
+        <v>1122</v>
       </c>
       <c r="J333" t="s">
         <v>75</v>
@@ -14086,28 +14506,31 @@
     </row>
     <row r="334" spans="1:10">
       <c r="A334" t="s">
-        <v>1058</v>
+        <v>1123</v>
+      </c>
+      <c r="B334" t="s">
+        <v>1124</v>
       </c>
       <c r="C334" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D334" t="s">
-        <v>870</v>
+        <v>874</v>
       </c>
       <c r="E334" t="s">
         <v>14</v>
       </c>
       <c r="F334" t="s">
-        <v>928</v>
+        <v>947</v>
       </c>
       <c r="G334" t="s">
-        <v>1059</v>
+        <v>1125</v>
       </c>
       <c r="H334" t="s">
-        <v>975</v>
+        <v>1010</v>
       </c>
       <c r="I334" t="s">
-        <v>993</v>
+        <v>1033</v>
       </c>
       <c r="J334" t="s">
         <v>75</v>
@@ -14115,19 +14538,22 @@
     </row>
     <row r="335" spans="1:10">
       <c r="A335" t="s">
-        <v>1060</v>
+        <v>1126</v>
+      </c>
+      <c r="B335" t="s">
+        <v>1127</v>
       </c>
       <c r="C335" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D335" t="s">
-        <v>1042</v>
+        <v>1102</v>
       </c>
       <c r="E335" t="s">
         <v>14</v>
       </c>
       <c r="F335" t="s">
-        <v>1061</v>
+        <v>1128</v>
       </c>
       <c r="G335" t="s">
         <v>24</v>
@@ -14144,28 +14570,31 @@
     </row>
     <row r="336" spans="1:10">
       <c r="A336" t="s">
-        <v>1062</v>
+        <v>1129</v>
+      </c>
+      <c r="B336" t="s">
+        <v>1130</v>
       </c>
       <c r="C336" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D336" t="s">
-        <v>900</v>
+        <v>911</v>
       </c>
       <c r="E336" t="s">
         <v>14</v>
       </c>
       <c r="F336" t="s">
-        <v>1063</v>
+        <v>1131</v>
       </c>
       <c r="G336" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="H336" t="s">
         <v>681</v>
       </c>
       <c r="I336" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="J336" t="s">
         <v>67</v>
@@ -14173,28 +14602,31 @@
     </row>
     <row r="337" spans="1:10">
       <c r="A337" t="s">
-        <v>1064</v>
+        <v>1132</v>
+      </c>
+      <c r="B337" t="s">
+        <v>1133</v>
       </c>
       <c r="C337" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D337" t="s">
-        <v>961</v>
+        <v>992</v>
       </c>
       <c r="E337" t="s">
         <v>14</v>
       </c>
       <c r="F337" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="G337" t="s">
-        <v>896</v>
+        <v>907</v>
       </c>
       <c r="H337" t="s">
         <v>647</v>
       </c>
       <c r="I337" t="s">
-        <v>1065</v>
+        <v>1134</v>
       </c>
       <c r="J337" t="s">
         <v>75</v>
@@ -14204,26 +14636,29 @@
       <c r="A338" t="s">
         <v>305</v>
       </c>
+      <c r="B338" t="s">
+        <v>1135</v>
+      </c>
       <c r="C338" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D338" t="s">
-        <v>1034</v>
+        <v>1091</v>
       </c>
       <c r="E338" t="s">
         <v>14</v>
       </c>
       <c r="F338" t="s">
-        <v>1066</v>
+        <v>1136</v>
       </c>
       <c r="G338" t="s">
-        <v>985</v>
+        <v>1023</v>
       </c>
       <c r="H338" t="s">
         <v>681</v>
       </c>
       <c r="I338" t="s">
-        <v>1067</v>
+        <v>1137</v>
       </c>
       <c r="J338" t="s">
         <v>91</v>
@@ -14231,28 +14666,31 @@
     </row>
     <row r="339" spans="1:10">
       <c r="A339" t="s">
-        <v>1068</v>
+        <v>1138</v>
+      </c>
+      <c r="B339" t="s">
+        <v>1139</v>
       </c>
       <c r="C339" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D339" t="s">
-        <v>1045</v>
+        <v>1106</v>
       </c>
       <c r="E339" t="s">
         <v>14</v>
       </c>
       <c r="F339" t="s">
-        <v>1069</v>
+        <v>1140</v>
       </c>
       <c r="G339" t="s">
-        <v>1070</v>
+        <v>1141</v>
       </c>
       <c r="H339" t="s">
-        <v>922</v>
+        <v>939</v>
       </c>
       <c r="I339" t="s">
-        <v>923</v>
+        <v>940</v>
       </c>
       <c r="J339" t="s">
         <v>91</v>
@@ -14260,22 +14698,25 @@
     </row>
     <row r="340" spans="1:10">
       <c r="A340" t="s">
-        <v>1071</v>
+        <v>1142</v>
+      </c>
+      <c r="B340" t="s">
+        <v>1143</v>
       </c>
       <c r="C340" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="D340" t="s">
-        <v>957</v>
+        <v>987</v>
       </c>
       <c r="E340" t="s">
         <v>14</v>
       </c>
       <c r="F340" t="s">
-        <v>916</v>
+        <v>932</v>
       </c>
       <c r="G340" t="s">
-        <v>1072</v>
+        <v>1144</v>
       </c>
       <c r="H340" t="s">
         <v>333</v>

</xml_diff>